<commit_message>
UC, DESC UC e check
</commit_message>
<xml_diff>
--- a/Documentação/Check List para apresentação/Check List Tarefas TCC II.xlsx
+++ b/Documentação/Check List para apresentação/Check List Tarefas TCC II.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>Check List -TCC II</t>
   </si>
@@ -206,13 +206,28 @@
   </si>
   <si>
     <t xml:space="preserve">   Relatório: Equipe e os dados da Proposta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1º Ativ: Submeter Correçao </t>
+  </si>
+  <si>
+    <t>Rel/proces: Porcentagem de Proposta AP e RP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2º Ativ: Corrigir proposta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1º Est: Status do Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2º Est: Status da Proposta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,8 +257,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +355,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -516,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -566,6 +593,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -650,6 +680,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -944,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O118"/>
+  <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -959,42 +991,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="19.5" thickBot="1">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="48"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="2:15">
       <c r="B3" s="1"/>
@@ -1003,55 +1035,55 @@
       <c r="B4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="3"/>
       <c r="I4" s="8" t="s">
         <v>46</v>
       </c>
       <c r="J4" s="9"/>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="2:15">
       <c r="B5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="4"/>
       <c r="I5" s="10" t="s">
         <v>48</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="38"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="39"/>
     </row>
     <row r="6" spans="2:15">
       <c r="B6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="4"/>
       <c r="I6" s="12" t="s">
         <v>54</v>
@@ -1059,205 +1091,205 @@
       <c r="J6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="36"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="38"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="39"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="4"/>
       <c r="I7" s="12"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="38"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="39"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="4"/>
       <c r="I8" s="13" t="s">
         <v>50</v>
       </c>
       <c r="J8" s="11"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="38"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="39"/>
     </row>
     <row r="9" spans="2:15">
       <c r="B9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="4"/>
       <c r="I9" s="12" t="s">
         <v>53</v>
       </c>
       <c r="J9" s="11"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="38"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="39"/>
     </row>
     <row r="10" spans="2:15">
       <c r="B10" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="4"/>
       <c r="I10" s="12" t="s">
         <v>52</v>
       </c>
       <c r="J10" s="11"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="38"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
     </row>
     <row r="11" spans="2:15">
       <c r="B11" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="4"/>
       <c r="I11" s="12" t="s">
         <v>51</v>
       </c>
       <c r="J11" s="11"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="38"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="39"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="4"/>
       <c r="I12" s="12" t="s">
         <v>47</v>
       </c>
       <c r="J12" s="11"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="38"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
     </row>
     <row r="13" spans="2:15">
       <c r="I13" s="12" t="s">
         <v>55</v>
       </c>
       <c r="J13" s="11"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="38"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="39"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55"/>
       <c r="H14" s="5"/>
       <c r="I14" s="12"/>
       <c r="J14" s="11"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="38"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58"/>
       <c r="H15" s="5"/>
       <c r="I15" s="13" t="s">
         <v>49</v>
       </c>
       <c r="J15" s="11"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="38"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" s="16"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="58"/>
       <c r="H16" s="5"/>
       <c r="I16" s="12" t="s">
         <v>56</v>
       </c>
       <c r="J16" s="11"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="38"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
       <c r="H17" s="5"/>
       <c r="I17" s="12" t="s">
         <v>57</v>
@@ -1265,1021 +1297,1047 @@
       <c r="J17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="38"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" s="16"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
       <c r="H18" s="5"/>
       <c r="I18" s="12"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="38"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="5"/>
       <c r="I19" s="12"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="38"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="39"/>
     </row>
     <row r="20" spans="2:15">
       <c r="B20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58"/>
       <c r="H20" s="5"/>
       <c r="I20" s="15"/>
       <c r="J20" s="14"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="41"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="42"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="2:15">
       <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="57"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="2:15">
       <c r="B23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="57"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="2:15">
       <c r="B24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="57"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="2:15">
       <c r="B25" s="16"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="57"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="58"/>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="2:15">
       <c r="B26" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="57"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="58"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" spans="2:15">
       <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="57"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="58"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="57"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="58"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:15">
       <c r="B29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="57"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="58"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="2:15">
       <c r="B30" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="57"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="2:15">
       <c r="B31" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="57"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="2:15">
       <c r="B32" s="16"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="57"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58"/>
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="55"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="57"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="58"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="16"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
-      <c r="G34" s="57"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="58"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="57"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="57"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="57"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="58"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="57"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="57"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="58"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="57"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="58"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="16"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="57"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="58"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="57"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="58"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="55"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="57"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="58"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="57"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="58"/>
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="57"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="58"/>
       <c r="H45" s="5"/>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="57"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="58"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="57"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="58"/>
       <c r="H47" s="5"/>
     </row>
     <row r="48" spans="2:8" ht="15" customHeight="1">
       <c r="B48" s="16"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="57"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="58"/>
       <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:8">
       <c r="B49" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="55"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="57"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="58"/>
       <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:8">
       <c r="B50" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="55"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="57"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="58"/>
       <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:8">
       <c r="B51" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="55"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="57"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="58"/>
       <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:8">
       <c r="B52" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="55"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="57"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="58"/>
       <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:8">
       <c r="B53" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="57"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="58"/>
       <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:8">
       <c r="B54" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="55"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="57"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="58"/>
       <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:8">
       <c r="B55" s="16"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="57"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="57"/>
+      <c r="G55" s="58"/>
       <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:8">
       <c r="B56" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="60"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="5"/>
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1">
       <c r="B58" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8">
       <c r="B59" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="39"/>
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" t="s">
+      <c r="A60" s="62" t="s">
         <v>59</v>
       </c>
       <c r="B60" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="39"/>
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" t="s">
+      <c r="A61" s="62" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" t="s">
+      <c r="A62" s="62" t="s">
         <v>59</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="39"/>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" t="s">
+      <c r="A63" s="62" t="s">
         <v>59</v>
       </c>
       <c r="B63" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" t="s">
+      <c r="A64" s="62" t="s">
         <v>59</v>
       </c>
       <c r="B64" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
       <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:8">
       <c r="B65" s="19"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="39"/>
       <c r="H65" s="4"/>
     </row>
     <row r="66" spans="1:8">
       <c r="B66" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="39"/>
       <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:8">
       <c r="B67" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="39"/>
       <c r="H67" s="4"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" t="s">
+      <c r="A68" s="63" t="s">
         <v>59</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
       <c r="H68" s="4"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" t="s">
+      <c r="A69" s="63" t="s">
         <v>59</v>
       </c>
       <c r="B69" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
       <c r="H69" s="4"/>
     </row>
     <row r="70" spans="1:8">
       <c r="B70" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="39"/>
       <c r="H70" s="4"/>
     </row>
     <row r="71" spans="1:8">
       <c r="B71" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="39"/>
       <c r="H71" s="4"/>
     </row>
     <row r="72" spans="1:8">
       <c r="B72" s="19"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="38"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="39"/>
       <c r="H72" s="4"/>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1">
       <c r="B73" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
       <c r="H73" s="4"/>
     </row>
     <row r="74" spans="1:8">
       <c r="B74" s="19"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
       <c r="H74" s="4"/>
     </row>
     <row r="75" spans="1:8">
       <c r="B75" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="37"/>
-      <c r="G75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="39"/>
       <c r="H75" s="4"/>
     </row>
     <row r="76" spans="1:8">
       <c r="B76" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="38"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="38"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="39"/>
       <c r="H76" s="4"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" t="s">
+      <c r="A77" s="63" t="s">
         <v>59</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="39"/>
       <c r="H77" s="4"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" t="s">
+      <c r="A78" s="63" t="s">
         <v>59</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="39"/>
       <c r="H78" s="4"/>
     </row>
     <row r="79" spans="1:8">
       <c r="B79" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
       <c r="H79" s="4"/>
     </row>
     <row r="80" spans="1:8">
       <c r="B80" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="33"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="B81" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="2:8">
-      <c r="B81" s="19"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="37"/>
-      <c r="G81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="39"/>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="2:8">
-      <c r="B82" s="19" t="s">
+    <row r="82" spans="1:8">
+      <c r="B82" s="19"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="B83" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="38"/>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="2:8">
-      <c r="B83" s="19" t="s">
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="4"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="B84" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="38"/>
-      <c r="H83" s="4"/>
-    </row>
-    <row r="84" spans="2:8">
-      <c r="B84" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="2:8">
+    <row r="85" spans="1:8">
+      <c r="A85" s="63" t="s">
+        <v>59</v>
+      </c>
       <c r="B85" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="38"/>
+        <v>64</v>
+      </c>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="39"/>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="2:8">
+    <row r="86" spans="1:8">
+      <c r="A86" s="63" t="s">
+        <v>59</v>
+      </c>
       <c r="B86" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="4"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="B87" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="4"/>
-    </row>
-    <row r="87" spans="2:8">
-      <c r="B87" s="19" t="s">
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="4"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="B88" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="4"/>
-    </row>
-    <row r="88" spans="2:8" ht="15" customHeight="1">
-      <c r="B88" s="19"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
-      <c r="G88" s="38"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="39"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="2:8">
-      <c r="B89" s="19" t="s">
+    <row r="89" spans="1:8" ht="15" customHeight="1">
+      <c r="B89" s="19"/>
+      <c r="C89" s="38"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="4"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="B90" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="37"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="37"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="4"/>
-    </row>
-    <row r="90" spans="2:8">
-      <c r="B90" s="19" t="s">
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="4"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="B91" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="4"/>
-    </row>
-    <row r="91" spans="2:8">
-      <c r="B91" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
-      <c r="G91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="2:8">
+    <row r="92" spans="1:8">
+      <c r="A92" s="63" t="s">
+        <v>59</v>
+      </c>
       <c r="B92" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C92" s="37"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="37"/>
-      <c r="G92" s="38"/>
+        <v>67</v>
+      </c>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="2:8">
+    <row r="93" spans="1:8">
+      <c r="A93" s="63" t="s">
+        <v>59</v>
+      </c>
       <c r="B93" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="4"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="B94" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C93" s="37"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="4"/>
-    </row>
-    <row r="94" spans="2:8">
-      <c r="B94" s="19" t="s">
+      <c r="C94" s="38"/>
+      <c r="D94" s="38"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="4"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="B95" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C94" s="37"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="4"/>
-    </row>
-    <row r="95" spans="2:8">
-      <c r="B95" s="19"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
-      <c r="G95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="39"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="2:8">
-      <c r="B96" s="19" t="s">
+    <row r="96" spans="1:8">
+      <c r="B96" s="19"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="38"/>
+      <c r="E96" s="38"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="39"/>
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B97" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="40"/>
-      <c r="F96" s="40"/>
-      <c r="G96" s="41"/>
-      <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="2:8">
-      <c r="B97" s="19"/>
-    </row>
-    <row r="98" spans="2:8">
-      <c r="B98" s="19" t="s">
+      <c r="C97" s="41"/>
+      <c r="D97" s="41"/>
+      <c r="E97" s="41"/>
+      <c r="F97" s="41"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="4"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="B98" s="19"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="B99" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="34" t="s">
+      <c r="C99" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D98" s="34"/>
-      <c r="E98" s="34"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="4"/>
-    </row>
-    <row r="99" spans="2:8">
-      <c r="B99" s="19"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
-      <c r="G99" s="38"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="35"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="2:8">
-      <c r="B100" s="19" t="s">
+    <row r="100" spans="1:8">
+      <c r="B100" s="19"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="39"/>
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="B101" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C100" s="37"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="4"/>
-    </row>
-    <row r="101" spans="2:8">
-      <c r="B101" s="19"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="38"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="38"/>
+      <c r="E101" s="38"/>
+      <c r="F101" s="38"/>
+      <c r="G101" s="39"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="2:8">
-      <c r="B102" s="20" t="s">
+    <row r="102" spans="1:8">
+      <c r="B102" s="19"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38"/>
+      <c r="G102" s="39"/>
+      <c r="H102" s="4"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="B103" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="40"/>
-      <c r="D102" s="40"/>
-      <c r="E102" s="40"/>
-      <c r="F102" s="40"/>
-      <c r="G102" s="41"/>
-      <c r="H102" s="4"/>
-    </row>
-    <row r="104" spans="2:8">
-      <c r="B104" s="30" t="s">
+      <c r="C103" s="41"/>
+      <c r="D103" s="41"/>
+      <c r="E103" s="41"/>
+      <c r="F103" s="41"/>
+      <c r="G103" s="42"/>
+      <c r="H103" s="4"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="B105" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="51"/>
-      <c r="D104" s="51"/>
-      <c r="E104" s="51"/>
-      <c r="F104" s="51"/>
-      <c r="G104" s="51"/>
-      <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="2:8">
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="2:8">
-      <c r="B106" s="27" t="s">
+      <c r="C105" s="52"/>
+      <c r="D105" s="52"/>
+      <c r="E105" s="52"/>
+      <c r="F105" s="52"/>
+      <c r="G105" s="52"/>
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="B107" s="27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="2:8">
-      <c r="B107" s="28" t="s">
+    <row r="108" spans="1:8">
+      <c r="B108" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="2:8">
-      <c r="B108" s="28" t="s">
+    <row r="109" spans="1:8">
+      <c r="B109" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="2:8">
-      <c r="B109" s="28" t="s">
+    <row r="110" spans="1:8">
+      <c r="B110" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="2:8">
-      <c r="B110" s="29" t="s">
+    <row r="111" spans="1:8">
+      <c r="B111" s="29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="2:8">
-      <c r="B112" s="6" t="s">
+    <row r="113" spans="2:2">
+      <c r="B113" s="6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2">
-      <c r="B113" s="31" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="114" spans="2:2">
       <c r="B114" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="115" spans="2:2">
       <c r="B115" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="116" spans="2:2">
       <c r="B116" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="117" spans="2:2">
       <c r="B117" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" s="31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="2:2">
-      <c r="B118" s="32" t="s">
+    <row r="119" spans="2:2">
+      <c r="B119" s="32" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2289,9 +2347,9 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="I2:O2"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="C58:G96"/>
-    <mergeCell ref="C98:G102"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="C58:G97"/>
+    <mergeCell ref="C99:G103"/>
     <mergeCell ref="C14:G56"/>
     <mergeCell ref="C4:G12"/>
   </mergeCells>

</xml_diff>